<commit_message>
Atualização de pesquisa_arquivos_sql.py - Organização de script - Atualização de funções de formatação - Atualização de função de percorrer lista de arquivo - Atualização de função de logger
On branch main
Your branch is up to date with 'origin/main'.

Changes to be committed:
	modified:   data/pesquisa_arquivos_sql/diretorios.xlsx
	renamed:    scripts/configurar_script.py -> scripts/configurar_path.py
	modified:   scripts/pesquisa_arquivos_sql.py
	modified:   utils/utils.py
</commit_message>
<xml_diff>
--- a/data/pesquisa_arquivos_sql/diretorios.xlsx
+++ b/data/pesquisa_arquivos_sql/diretorios.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Auto Service</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Z:\AutoService\000_CRM\db\scripts\</t>
   </si>
   <si>
@@ -104,6 +101,12 @@
   </si>
   <si>
     <t>Z:\Unilever\003_NOLA\db\scripts\</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>C:\Users\rapha\Desktop\Input_Python\scripts_auto_service</t>
   </si>
 </sst>
 </file>
@@ -140,12 +143,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -166,8 +166,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C13" displayName="Table1" name="Table1" id="1" totalsRowShown="0">
-  <autoFilter ref="A1:C13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C14" displayName="Table1" name="Table1" id="1" totalsRowShown="0">
+  <autoFilter ref="A1:C14"/>
   <tableColumns count="3">
     <tableColumn name="CLIENTE" id="1" totalsRowLabel="Total"/>
     <tableColumn name="PASTA" id="2"/>
@@ -175,7 +175,7 @@
       <totalsRowFormula>Sum</totalsRowFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
+  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
 </table>
 </file>
 
@@ -467,15 +467,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="45.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="57.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -515,110 +515,107 @@
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="1" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>